<commit_message>
naceneni 0.6, zduvodneni nakladu
</commit_message>
<xml_diff>
--- a/grant_naceneni.xlsx
+++ b/grant_naceneni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t xml:space="preserve">Městská senzorická síť – cenový odhad</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t xml:space="preserve">HackRF One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MacBook Pro 13" Retina CZ 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.alza.cz/macbook-pro-13-retina-cz-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dell Latitude E5470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.alza.cz/dell-latitude-e5470-d4270193.htm?catid=18853299</t>
   </si>
   <si>
     <t xml:space="preserve">suma celkem za jasně odhadnutelné položky</t>
@@ -525,7 +549,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,11 +573,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -561,7 +585,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,10 +718,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -770,7 +794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -808,7 +832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
@@ -846,7 +870,7 @@
       </c>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -884,7 +908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -922,7 +946,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
@@ -958,7 +982,7 @@
       </c>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>28</v>
       </c>
@@ -995,7 +1019,7 @@
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
@@ -1032,7 +1056,7 @@
       </c>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>32</v>
       </c>
@@ -1071,7 +1095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>34</v>
       </c>
@@ -1109,7 +1133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>37</v>
       </c>
@@ -1145,7 +1169,7 @@
       </c>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
@@ -1184,7 +1208,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
         <v>41</v>
       </c>
@@ -1221,7 +1245,7 @@
       </c>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
         <v>43</v>
       </c>
@@ -1258,115 +1282,153 @@
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
+    <row r="16" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19" t="n">
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="9" t="n">
+        <f aca="false">C16*E16</f>
+        <v>39990</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="n">
+        <f aca="false">F16+G16</f>
+        <v>39990</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <f aca="false">F16+G16</f>
+        <v>39990</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <f aca="false">C17*E17</f>
+        <v>35690</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="n">
+        <f aca="false">F17+G17</f>
+        <v>35690</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <f aca="false">F17+G17</f>
+        <v>35690</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19" t="n">
         <f aca="false">SUM(F3:F15)</f>
         <v>1115270</v>
       </c>
-      <c r="G16" s="19" t="n">
+      <c r="G18" s="19" t="n">
         <f aca="false">SUM(G3:G15)</f>
         <v>165908</v>
       </c>
-      <c r="H16" s="19" t="n">
-        <f aca="false">SUM(F16:G16)</f>
+      <c r="H18" s="19" t="n">
+        <f aca="false">SUM(F18:G18)</f>
         <v>1281178</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="20" t="n">
-        <f aca="false">SUM(J3:J15)</f>
-        <v>1316067</v>
-      </c>
-      <c r="K16" s="19" t="n">
-        <f aca="false">SUM(K3:K15)</f>
-        <v>1316067</v>
-      </c>
-      <c r="L16" s="18"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="I18" s="18"/>
+      <c r="J18" s="20" t="n">
+        <f aca="false">SUM(J3:J17)</f>
+        <v>1391747</v>
+      </c>
+      <c r="K18" s="19" t="n">
+        <f aca="false">SUM(K3:K17)</f>
+        <v>1391747</v>
+      </c>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="23" t="n">
+      <c r="C19" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23" t="n">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23" t="n">
         <v>500000</v>
       </c>
-      <c r="G17" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22" t="n">
-        <f aca="false">F17+G17</f>
+      <c r="G19" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22" t="n">
+        <f aca="false">F19+G19</f>
         <v>500000</v>
       </c>
-      <c r="L17" s="22"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="L19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
@@ -1380,17 +1442,17 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+        <v>56</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -1400,13 +1462,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -1420,13 +1482,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -1438,15 +1500,15 @@
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
     </row>
-    <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -1458,15 +1520,15 @@
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -1478,15 +1540,15 @@
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -1498,15 +1560,15 @@
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
-        <v>57</v>
+    <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -1518,15 +1580,15 @@
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -1540,116 +1602,156 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="11" t="n">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="11"/>
-      <c r="E29" s="11" t="n">
-        <v>50000</v>
-      </c>
-      <c r="F29" s="11" t="n">
-        <v>50000</v>
-      </c>
-      <c r="G29" s="11" t="n">
-        <v>50000</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>62</v>
+    <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-      <c r="H30" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="28" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="25" t="n">
+      <c r="C31" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="D31" s="25" t="n">
-        <v>107500</v>
-      </c>
-      <c r="E31" s="25" t="n">
-        <v>107500</v>
-      </c>
-      <c r="F31" s="25" t="n">
-        <v>107500</v>
-      </c>
-      <c r="G31" s="25" t="n">
-        <v>0</v>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11" t="n">
+        <v>50000</v>
+      </c>
+      <c r="F31" s="11" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G31" s="11" t="n">
+        <v>50000</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
-      <c r="L31" s="28" t="s">
-        <v>67</v>
-      </c>
+      <c r="L31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19" t="n">
-        <f aca="false">SUM(F3:F19)</f>
-        <v>2730540</v>
-      </c>
-      <c r="G32" s="19" t="n">
-        <f aca="false">SUM(G3:G19)</f>
+      <c r="A32" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="25" t="n">
+        <v>107500</v>
+      </c>
+      <c r="E33" s="25" t="n">
+        <v>107500</v>
+      </c>
+      <c r="F33" s="25" t="n">
+        <v>107500</v>
+      </c>
+      <c r="G33" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19" t="n">
+        <f aca="false">SUM(F3:F21)</f>
+        <v>2806220</v>
+      </c>
+      <c r="G34" s="19" t="n">
+        <f aca="false">SUM(G3:G21)</f>
         <v>331816</v>
       </c>
-      <c r="H32" s="19" t="n">
-        <f aca="false">SUM(F32:G32)</f>
-        <v>3062356</v>
-      </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="20" t="n">
+      <c r="H34" s="19" t="n">
+        <f aca="false">SUM(F34:G34)</f>
+        <v>3138036</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="20" t="n">
         <f aca="false">SUM(J3:J15)</f>
         <v>1316067</v>
       </c>
-      <c r="K32" s="29" t="n">
-        <f aca="false">SUM(K16:K17)</f>
-        <v>1816067</v>
-      </c>
-      <c r="L32" s="18"/>
+      <c r="K34" s="29" t="n">
+        <f aca="false">SUM(K18:K19)</f>
+        <v>1891747</v>
+      </c>
+      <c r="L34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
formatovani pro pdf, oprava pocitani souctu celkem za vse
</commit_message>
<xml_diff>
--- a/grant_naceneni.xlsx
+++ b/grant_naceneni.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
   <si>
     <t>Městská senzorická síť – cenový odhad</t>
   </si>
@@ -232,9 +232,6 @@
     <t xml:space="preserve"> - pronájem letiště na testování drona</t>
   </si>
   <si>
-    <t xml:space="preserve"> - kalibrace různých senzorů v laboratorních laboratoři</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - speciální software pro pen-testing celého systému a NB-IoT</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve"> - komerční varianty například Smart Cities PRO fi Libelium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - kalibrace různých senzorů v laboratorních podmínkách</t>
   </si>
 </sst>
 </file>
@@ -275,12 +275,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00,&quot;Kč&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -386,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -561,15 +568,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -582,128 +585,254 @@
       <right style="double">
         <color auto="1"/>
       </right>
-      <top style="double">
-        <color auto="1"/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1079,20 +1208,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AMH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="68.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1"/>
+    <col min="2" max="2" width="5.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.140625" style="1"/>
-    <col min="4" max="5" width="11.5703125" style="1"/>
-    <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1103,1330 +1237,1325 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+    </row>
+    <row r="2" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="61" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="47">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="47">
         <v>47768</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="47">
         <v>57799</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="47">
         <v>57799</v>
       </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="18">
-        <v>0</v>
-      </c>
-      <c r="I3" s="23">
+      <c r="G3" s="48">
+        <v>0</v>
+      </c>
+      <c r="H3" s="49">
+        <v>0</v>
+      </c>
+      <c r="I3" s="50">
         <f>F3+G3+H3</f>
         <v>57799</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="51">
         <f>G3+H3+I3</f>
         <v>57799</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>12</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>3350</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>4053</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <f>E4*12</f>
         <v>48636</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <f>C4*E4</f>
         <v>48636</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <f>C4*E4</f>
         <v>48636</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="21">
         <f t="shared" ref="I4:I15" si="0">F4+G4+H4</f>
         <v>145908</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="22">
         <f t="shared" ref="J4:J15" si="1">F4+G4+H4</f>
         <v>145908</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="5"/>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
         <v>200000</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>200000</v>
       </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="18">
-        <v>0</v>
-      </c>
-      <c r="I5" s="23">
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="22">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>500</v>
       </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
         <v>1000</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <f>C6*E6</f>
         <v>500000</v>
       </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="18">
-        <v>0</v>
-      </c>
-      <c r="I6" s="23">
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="22">
         <f t="shared" si="1"/>
         <v>500000</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="48" t="s">
+      <c r="M6" s="38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>100</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
         <v>1000</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <f>C7*E7</f>
         <v>100000</v>
       </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="23">
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="22">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>100</v>
       </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
         <v>1000</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>50000</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>50000</v>
       </c>
-      <c r="H8" s="18">
-        <v>0</v>
-      </c>
-      <c r="I8" s="23">
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="22">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="21">
         <f t="shared" si="0"/>
         <v>48780</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="22">
         <f t="shared" si="1"/>
         <v>48780</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>1</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
         <v>15790</v>
       </c>
-      <c r="G10" s="7">
-        <v>0</v>
-      </c>
-      <c r="H10" s="20">
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="18">
         <v>15790</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="21">
         <f t="shared" si="0"/>
         <v>31580</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="22">
         <f t="shared" si="1"/>
         <v>31580</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="7"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>27490</v>
       </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
         <f>C11*H11</f>
         <v>22719</v>
       </c>
-      <c r="G11" s="7">
-        <v>0</v>
-      </c>
-      <c r="H11" s="20">
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="18">
         <v>22719</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="21">
         <f t="shared" si="0"/>
         <v>45438</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="22">
         <f t="shared" si="1"/>
         <v>45438</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>7500</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>7500</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <f>C12*E12</f>
         <v>15000</v>
       </c>
-      <c r="G12" s="7">
-        <v>0</v>
-      </c>
-      <c r="H12" s="18">
-        <v>0</v>
-      </c>
-      <c r="I12" s="23">
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="22">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>7418</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>7418</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <f>C13*E13</f>
         <v>14836</v>
       </c>
-      <c r="G13" s="7">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
-        <v>0</v>
-      </c>
-      <c r="I13" s="23">
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
         <f t="shared" si="0"/>
         <v>14836</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="22">
         <f t="shared" si="1"/>
         <v>14836</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12" t="s">
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="18">
-        <v>0</v>
-      </c>
-      <c r="I14" s="23">
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
         <f t="shared" si="0"/>
         <v>39990</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="22">
         <f t="shared" si="1"/>
         <v>39990</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>1</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="4">
         <f>C15*E15</f>
         <v>35690</v>
       </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0</v>
-      </c>
-      <c r="I15" s="33">
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="28">
         <f t="shared" si="0"/>
         <v>35690</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="29">
         <f t="shared" si="1"/>
         <v>35690</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29">
+      <c r="B16" s="43"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24">
         <f>SUM(F3:F15)</f>
         <v>1060470</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="24">
         <f>SUM(G3:G15)</f>
         <v>98636</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="25">
         <f>SUM(H3:H15)</f>
         <v>87145</v>
       </c>
-      <c r="I16" s="37">
+      <c r="I16" s="32">
         <f>SUM(I3:I15)</f>
         <v>1335021</v>
       </c>
-      <c r="J16" s="38">
+      <c r="J16" s="33">
         <f>SUM(J3:J15)</f>
         <v>1335021</v>
       </c>
-      <c r="K16" s="31"/>
-      <c r="L16" s="32">
-        <f>SUM(F16:G16)</f>
-        <v>1159106</v>
-      </c>
-      <c r="M16" s="28"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="23"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="14">
         <v>1</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14">
         <v>500000</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="14">
         <v>500000</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="14">
         <v>500000</v>
       </c>
-      <c r="I17" s="35">
-        <v>0</v>
-      </c>
-      <c r="J17" s="36">
+      <c r="I17" s="30">
+        <v>0</v>
+      </c>
+      <c r="J17" s="31">
         <v>500000</v>
       </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="15" t="s">
+      <c r="K17" s="20"/>
+      <c r="L17" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="17">
-        <v>0</v>
-      </c>
-      <c r="H18" s="18">
-        <v>0</v>
-      </c>
-      <c r="I18" s="23">
-        <v>0</v>
-      </c>
-      <c r="J18" s="24">
-        <v>0</v>
-      </c>
-      <c r="K18" s="21" t="s">
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
+        <v>0</v>
+      </c>
+      <c r="J18" s="22">
+        <v>0</v>
+      </c>
+      <c r="K18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0</v>
-      </c>
-      <c r="I19" s="23">
-        <v>0</v>
-      </c>
-      <c r="J19" s="24">
-        <v>0</v>
-      </c>
-      <c r="K19" s="21" t="s">
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="16">
+        <v>0</v>
+      </c>
+      <c r="I19" s="21">
+        <v>0</v>
+      </c>
+      <c r="J19" s="22">
+        <v>0</v>
+      </c>
+      <c r="K19" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+      <c r="H20" s="16">
+        <v>0</v>
+      </c>
+      <c r="I20" s="21">
+        <v>0</v>
+      </c>
+      <c r="J20" s="22">
+        <v>0</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0</v>
-      </c>
-      <c r="I20" s="23">
-        <v>0</v>
-      </c>
-      <c r="J20" s="24">
-        <v>0</v>
-      </c>
-      <c r="K20" s="21" t="s">
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0</v>
+      </c>
+      <c r="I21" s="21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="22">
+        <v>0</v>
+      </c>
+      <c r="K21" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="17">
-        <v>0</v>
-      </c>
-      <c r="H21" s="18">
-        <v>0</v>
-      </c>
-      <c r="I21" s="23">
-        <v>0</v>
-      </c>
-      <c r="J21" s="24">
-        <v>0</v>
-      </c>
-      <c r="K21" s="21" t="s">
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0</v>
+      </c>
+      <c r="I22" s="21">
+        <v>0</v>
+      </c>
+      <c r="J22" s="22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="7">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0</v>
-      </c>
-      <c r="G22" s="17">
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <v>0</v>
-      </c>
-      <c r="I22" s="23">
-        <v>0</v>
-      </c>
-      <c r="J22" s="24">
-        <v>0</v>
-      </c>
-      <c r="K22" s="21" t="s">
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21">
+        <v>0</v>
+      </c>
+      <c r="J23" s="22">
+        <v>0</v>
+      </c>
+      <c r="K23" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="17">
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="24">
-        <v>0</v>
-      </c>
-      <c r="K23" s="21" t="s">
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="15">
+        <v>0</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+      <c r="I24" s="21">
+        <v>0</v>
+      </c>
+      <c r="J24" s="22">
+        <v>0</v>
+      </c>
+      <c r="K24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="7">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7">
-        <v>0</v>
-      </c>
-      <c r="G24" s="17">
-        <v>0</v>
-      </c>
-      <c r="H24" s="18">
-        <v>0</v>
-      </c>
-      <c r="I24" s="23">
-        <v>0</v>
-      </c>
-      <c r="J24" s="24">
-        <v>0</v>
-      </c>
-      <c r="K24" s="21" t="s">
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="15">
+        <v>0</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+      <c r="I25" s="21">
+        <v>0</v>
+      </c>
+      <c r="J25" s="22">
+        <v>0</v>
+      </c>
+      <c r="K25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="7">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7">
-        <v>0</v>
-      </c>
-      <c r="G25" s="17">
-        <v>0</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="23">
-        <v>0</v>
-      </c>
-      <c r="J25" s="24">
-        <v>0</v>
-      </c>
-      <c r="K25" s="21" t="s">
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
+      <c r="J26" s="22">
+        <v>0</v>
+      </c>
+      <c r="K26" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="7">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0</v>
-      </c>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="23">
-        <v>0</v>
-      </c>
-      <c r="J26" s="24">
-        <v>0</v>
-      </c>
-      <c r="K26" s="21" t="s">
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="15">
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="I27" s="21">
+        <v>0</v>
+      </c>
+      <c r="J27" s="22">
+        <v>0</v>
+      </c>
+      <c r="K27" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0</v>
-      </c>
-      <c r="G27" s="17">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="23">
-        <v>0</v>
-      </c>
-      <c r="J27" s="24">
-        <v>0</v>
-      </c>
-      <c r="K27" s="21" t="s">
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="21">
+        <v>0</v>
+      </c>
+      <c r="J28" s="22">
+        <v>0</v>
+      </c>
+      <c r="K28" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="17">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="23">
-        <v>0</v>
-      </c>
-      <c r="J28" s="24">
-        <v>0</v>
-      </c>
-      <c r="K28" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
+      <c r="B29" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>50000</v>
+      </c>
+      <c r="F29" s="5">
+        <v>50000</v>
+      </c>
+      <c r="G29" s="15">
+        <v>50000</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0</v>
+      </c>
+      <c r="I29" s="21">
+        <v>0</v>
+      </c>
+      <c r="J29" s="22">
+        <v>0</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="15">
+        <v>0</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0</v>
+      </c>
+      <c r="I30" s="21">
+        <v>0</v>
+      </c>
+      <c r="J30" s="22">
+        <v>0</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>50000</v>
-      </c>
-      <c r="F29" s="7">
-        <v>50000</v>
-      </c>
-      <c r="G29" s="17">
-        <v>50000</v>
-      </c>
-      <c r="H29" s="18">
-        <v>0</v>
-      </c>
-      <c r="I29" s="23">
-        <v>0</v>
-      </c>
-      <c r="J29" s="24">
-        <v>0</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="M29" s="7"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="17">
-        <v>0</v>
-      </c>
-      <c r="H30" s="18">
-        <v>0</v>
-      </c>
-      <c r="I30" s="23">
-        <v>0</v>
-      </c>
-      <c r="J30" s="24">
-        <v>0</v>
-      </c>
-      <c r="K30" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M30" s="7"/>
-    </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="6">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>33462.81</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="4">
         <v>40490</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="4">
         <v>40490</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="5">
         <v>20000</v>
       </c>
-      <c r="H31" s="18">
-        <v>0</v>
-      </c>
-      <c r="I31" s="23">
+      <c r="H31" s="16">
+        <v>0</v>
+      </c>
+      <c r="I31" s="21">
         <f>C31+D31</f>
         <v>33463.81</v>
       </c>
-      <c r="J31" s="24">
+      <c r="J31" s="22">
         <f>F31+G31</f>
         <v>60490</v>
       </c>
-      <c r="K31" s="21" t="s">
+      <c r="K31" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="7" t="s">
+      <c r="L31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M31" s="5" t="s">
+      <c r="M31" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="4">
         <v>1</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="7">
-        <v>0</v>
-      </c>
-      <c r="H32" s="18">
-        <v>0</v>
-      </c>
-      <c r="I32" s="23">
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="16">
+        <v>0</v>
+      </c>
+      <c r="I32" s="21">
         <f>C32+D32</f>
         <v>8678</v>
       </c>
-      <c r="J32" s="24">
+      <c r="J32" s="22">
         <f>F32+G32</f>
         <v>10499</v>
       </c>
-      <c r="K32" s="21" t="s">
+      <c r="K32" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L32" s="7" t="s">
+      <c r="L32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="5"/>
+      <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="4">
         <v>1</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="4">
         <v>107500</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="4">
         <v>107500</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="4">
         <v>107500</v>
       </c>
-      <c r="G33" s="6">
-        <v>0</v>
-      </c>
-      <c r="H33" s="18">
-        <v>0</v>
-      </c>
-      <c r="I33" s="33">
-        <v>0</v>
-      </c>
-      <c r="J33" s="34">
-        <v>0</v>
-      </c>
-      <c r="K33" s="21" t="s">
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="16">
+        <v>0</v>
+      </c>
+      <c r="I33" s="28">
+        <v>0</v>
+      </c>
+      <c r="J33" s="29">
+        <v>0</v>
+      </c>
+      <c r="K33" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="7" t="s">
+      <c r="L33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="M33" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29">
+      <c r="B34" s="43"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24">
         <f>SUM(F16:F17)</f>
         <v>1560470</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="24">
         <f>SUM(G16:G17)</f>
         <v>598636</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="24">
         <f>SUM(H16:H17)</f>
         <v>587145</v>
       </c>
-      <c r="I34" s="39">
+      <c r="I34" s="34">
         <f>SUM(I16:I33)</f>
         <v>1377162.81</v>
       </c>
-      <c r="J34" s="40">
-        <f>SUM(J16:J33)</f>
-        <v>1906010</v>
-      </c>
-      <c r="K34" s="31"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="28"/>
+      <c r="J34" s="35">
+        <f>J16+J17</f>
+        <v>1835021</v>
+      </c>
+      <c r="K34" s="26"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="23"/>
     </row>
     <row r="35" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -2436,8 +2565,8 @@
   <hyperlinks>
     <hyperlink ref="M6" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="82" fitToWidth="0" orientation="landscape" useFirstPageNumber="1" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
final naceneni, i v pdf, ver 1.0
</commit_message>
<xml_diff>
--- a/grant_naceneni.xlsx
+++ b/grant_naceneni.xlsx
@@ -275,12 +275,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00,&quot;Kč&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -345,7 +352,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,8 +399,14 @@
         <fgColor theme="7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -552,19 +565,6 @@
       <bottom style="double">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -633,10 +633,86 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -646,14 +722,70 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color auto="1"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -664,11 +796,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -676,168 +808,240 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="27" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="28" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="30" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="33" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
     <cellStyle name="Accent4" xfId="4" builtinId="41"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -1211,10 +1415,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMH35"/>
+  <dimension ref="A1:AMH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1237,1327 +1441,1326 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="61" t="s">
+      <c r="M2" s="53" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="31">
         <v>1</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="31">
         <v>47768</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="31">
         <v>57799</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="31">
         <v>57799</v>
       </c>
-      <c r="G3" s="48">
-        <v>0</v>
-      </c>
-      <c r="H3" s="49">
-        <v>0</v>
-      </c>
-      <c r="I3" s="50">
+      <c r="G3" s="32">
+        <v>0</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0</v>
+      </c>
+      <c r="I3" s="38">
         <f>F3+G3+H3</f>
         <v>57799</v>
       </c>
-      <c r="J3" s="51">
+      <c r="J3" s="34">
         <f>G3+H3+I3</f>
         <v>57799</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="55" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>12</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>3350</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>4053</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f>E4*12</f>
         <v>48636</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <f>C4*E4</f>
         <v>48636</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="10">
         <f>C4*E4</f>
         <v>48636</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="39">
         <f t="shared" ref="I4:I15" si="0">F4+G4+H4</f>
         <v>145908</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="16">
         <f t="shared" ref="J4:J15" si="1">F4+G4+H4</f>
         <v>145908</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="3"/>
+      <c r="M4" s="55"/>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>200000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>200000</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16">
-        <v>0</v>
-      </c>
-      <c r="I5" s="21">
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="39">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="16">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="55" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>500</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>1000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <f>C6*E6</f>
         <v>500000</v>
       </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16">
-        <v>0</v>
-      </c>
-      <c r="I6" s="21">
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="39">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="16">
         <f t="shared" si="1"/>
         <v>500000</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="58" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>100</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
         <v>1000</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <f>C7*E7</f>
         <v>100000</v>
       </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="39">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="16">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="55"/>
     </row>
     <row r="8" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>100</v>
       </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
         <v>1000</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>50000</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>50000</v>
       </c>
-      <c r="H8" s="16">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21">
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="39">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="16">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="3"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17" t="s">
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="39">
         <f t="shared" si="0"/>
         <v>48780</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="16">
         <f t="shared" si="1"/>
         <v>48780</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="55" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <v>15790</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="18">
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
         <v>15790</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="39">
         <f t="shared" si="0"/>
         <v>31580</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="16">
         <f t="shared" si="1"/>
         <v>31580</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="5"/>
+      <c r="M10" s="60"/>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>1</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>27490</v>
       </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <f>C11*H11</f>
         <v>22719</v>
       </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="18">
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12">
         <v>22719</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="39">
         <f t="shared" si="0"/>
         <v>45438</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="16">
         <f t="shared" si="1"/>
         <v>45438</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="60" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>7500</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>7500</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="2">
         <f>C12*E12</f>
         <v>15000</v>
       </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="39">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="16">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="5"/>
+      <c r="M12" s="60"/>
     </row>
     <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>7418</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>7418</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="2">
         <f>C13*E13</f>
         <v>14836</v>
       </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="16">
-        <v>0</v>
-      </c>
-      <c r="I13" s="21">
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="39">
         <f t="shared" si="0"/>
         <v>14836</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="16">
         <f t="shared" si="1"/>
         <v>14836</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="5"/>
+      <c r="M13" s="60"/>
     </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>1</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="16">
-        <v>0</v>
-      </c>
-      <c r="I14" s="21">
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="39">
         <f t="shared" si="0"/>
         <v>39990</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="16">
         <f t="shared" si="1"/>
         <v>39990</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="60" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="2">
         <f>C15*E15</f>
         <v>35690</v>
       </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0</v>
-      </c>
-      <c r="I15" s="28">
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="40">
         <f t="shared" si="0"/>
         <v>35690</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="22">
         <f t="shared" si="1"/>
         <v>35690</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="60" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24">
+      <c r="B16" s="28"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17">
         <f>SUM(F3:F15)</f>
         <v>1060470</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="17">
         <f>SUM(G3:G15)</f>
         <v>98636</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="18">
         <f>SUM(H3:H15)</f>
         <v>87145</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="25">
         <f>SUM(I3:I15)</f>
         <v>1335021</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="26">
         <f>SUM(J3:J15)</f>
         <v>1335021</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="23"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="63"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
         <v>500000</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="8">
         <v>500000</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="8">
         <v>500000</v>
       </c>
-      <c r="I17" s="30">
-        <v>0</v>
-      </c>
-      <c r="J17" s="31">
+      <c r="I17" s="23">
+        <v>0</v>
+      </c>
+      <c r="J17" s="24">
         <v>500000</v>
       </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="13" t="s">
+      <c r="K17" s="14"/>
+      <c r="L17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="13"/>
+      <c r="M17" s="65"/>
     </row>
     <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="15">
-        <v>0</v>
-      </c>
-      <c r="H18" s="16">
-        <v>0</v>
-      </c>
-      <c r="I18" s="21">
-        <v>0</v>
-      </c>
-      <c r="J18" s="22">
-        <v>0</v>
-      </c>
-      <c r="K18" s="19" t="s">
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0</v>
+      </c>
+      <c r="J18" s="36">
+        <v>0</v>
+      </c>
+      <c r="K18" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="60"/>
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0</v>
-      </c>
-      <c r="G19" s="15">
-        <v>0</v>
-      </c>
-      <c r="H19" s="16">
-        <v>0</v>
-      </c>
-      <c r="I19" s="21">
-        <v>0</v>
-      </c>
-      <c r="J19" s="22">
-        <v>0</v>
-      </c>
-      <c r="K19" s="19" t="s">
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
+      <c r="J19" s="36">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="60"/>
     </row>
     <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="5">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="15">
-        <v>0</v>
-      </c>
-      <c r="H20" s="16">
-        <v>0</v>
-      </c>
-      <c r="I20" s="21">
-        <v>0</v>
-      </c>
-      <c r="J20" s="22">
-        <v>0</v>
-      </c>
-      <c r="K20" s="19" t="s">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0</v>
+      </c>
+      <c r="J20" s="36">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="60"/>
     </row>
     <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="5">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0</v>
-      </c>
-      <c r="H21" s="16">
-        <v>0</v>
-      </c>
-      <c r="I21" s="21">
-        <v>0</v>
-      </c>
-      <c r="J21" s="22">
-        <v>0</v>
-      </c>
-      <c r="K21" s="19" t="s">
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="36">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="60"/>
     </row>
     <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="5">
-        <v>0</v>
-      </c>
-      <c r="E22" s="5">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0</v>
-      </c>
-      <c r="I22" s="21">
-        <v>0</v>
-      </c>
-      <c r="J22" s="22">
-        <v>0</v>
-      </c>
-      <c r="K22" s="19" t="s">
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="36">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="60"/>
     </row>
     <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="15">
-        <v>0</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0</v>
-      </c>
-      <c r="I23" s="21">
-        <v>0</v>
-      </c>
-      <c r="J23" s="22">
-        <v>0</v>
-      </c>
-      <c r="K23" s="19" t="s">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0</v>
+      </c>
+      <c r="J23" s="36">
+        <v>0</v>
+      </c>
+      <c r="K23" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="60"/>
     </row>
     <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
-        <v>0</v>
-      </c>
-      <c r="G24" s="15">
-        <v>0</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0</v>
-      </c>
-      <c r="I24" s="21">
-        <v>0</v>
-      </c>
-      <c r="J24" s="22">
-        <v>0</v>
-      </c>
-      <c r="K24" s="19" t="s">
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0</v>
+      </c>
+      <c r="J24" s="36">
+        <v>0</v>
+      </c>
+      <c r="K24" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="60"/>
     </row>
     <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0</v>
-      </c>
-      <c r="G25" s="15">
-        <v>0</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0</v>
-      </c>
-      <c r="I25" s="21">
-        <v>0</v>
-      </c>
-      <c r="J25" s="22">
-        <v>0</v>
-      </c>
-      <c r="K25" s="19" t="s">
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="15">
+        <v>0</v>
+      </c>
+      <c r="J25" s="36">
+        <v>0</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="60"/>
     </row>
     <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="15">
-        <v>0</v>
-      </c>
-      <c r="H26" s="16">
-        <v>0</v>
-      </c>
-      <c r="I26" s="21">
-        <v>0</v>
-      </c>
-      <c r="J26" s="22">
-        <v>0</v>
-      </c>
-      <c r="K26" s="19" t="s">
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="36">
+        <v>0</v>
+      </c>
+      <c r="K26" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="60"/>
     </row>
     <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="G27" s="15">
-        <v>0</v>
-      </c>
-      <c r="H27" s="16">
-        <v>0</v>
-      </c>
-      <c r="I27" s="21">
-        <v>0</v>
-      </c>
-      <c r="J27" s="22">
-        <v>0</v>
-      </c>
-      <c r="K27" s="19" t="s">
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0</v>
+      </c>
+      <c r="J27" s="36">
+        <v>0</v>
+      </c>
+      <c r="K27" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="60"/>
     </row>
     <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
-      </c>
-      <c r="G28" s="15">
-        <v>0</v>
-      </c>
-      <c r="H28" s="16">
-        <v>0</v>
-      </c>
-      <c r="I28" s="21">
-        <v>0</v>
-      </c>
-      <c r="J28" s="22">
-        <v>0</v>
-      </c>
-      <c r="K28" s="19" t="s">
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0</v>
+      </c>
+      <c r="J28" s="36">
+        <v>0</v>
+      </c>
+      <c r="K28" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="60"/>
     </row>
     <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="3">
         <v>1</v>
       </c>
-      <c r="D29" s="5">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5">
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
         <v>50000</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="3">
         <v>50000</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="9">
         <v>50000</v>
       </c>
-      <c r="H29" s="16">
-        <v>0</v>
-      </c>
-      <c r="I29" s="21">
-        <v>0</v>
-      </c>
-      <c r="J29" s="22">
-        <v>0</v>
-      </c>
-      <c r="K29" s="19" t="s">
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0</v>
+      </c>
+      <c r="J29" s="36">
+        <v>0</v>
+      </c>
+      <c r="K29" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M29" s="5"/>
+      <c r="M29" s="60"/>
     </row>
     <row r="30" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5">
-        <v>0</v>
-      </c>
-      <c r="G30" s="15">
-        <v>0</v>
-      </c>
-      <c r="H30" s="16">
-        <v>0</v>
-      </c>
-      <c r="I30" s="21">
-        <v>0</v>
-      </c>
-      <c r="J30" s="22">
-        <v>0</v>
-      </c>
-      <c r="K30" s="19" t="s">
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="36">
+        <v>0</v>
+      </c>
+      <c r="K30" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="M30" s="5"/>
+      <c r="M30" s="60"/>
     </row>
     <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="2">
         <v>1</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="2">
         <v>33462.81</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <v>40490</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="2">
         <v>40490</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="3">
         <v>20000</v>
       </c>
-      <c r="H31" s="16">
-        <v>0</v>
-      </c>
-      <c r="I31" s="21">
+      <c r="H31" s="10">
+        <v>0</v>
+      </c>
+      <c r="I31" s="15">
         <f>C31+D31</f>
         <v>33463.81</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="36">
         <f>F31+G31</f>
         <v>60490</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="L31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="55" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="16">
-        <v>0</v>
-      </c>
-      <c r="I32" s="21">
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+      <c r="I32" s="15">
         <f>C32+D32</f>
         <v>8678</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="36">
         <f>F32+G32</f>
         <v>10499</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="L32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="3"/>
+      <c r="M32" s="55"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="2">
         <v>1</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>107500</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <v>107500</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="2">
         <v>107500</v>
       </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
-      <c r="H33" s="16">
-        <v>0</v>
-      </c>
-      <c r="I33" s="28">
-        <v>0</v>
-      </c>
-      <c r="J33" s="29">
-        <v>0</v>
-      </c>
-      <c r="K33" s="19" t="s">
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0</v>
+      </c>
+      <c r="I33" s="21">
+        <v>0</v>
+      </c>
+      <c r="J33" s="37">
+        <v>0</v>
+      </c>
+      <c r="K33" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="L33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="M33" s="55" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24">
+      <c r="B34" s="70"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71">
         <f>SUM(F16:F17)</f>
         <v>1560470</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="71">
         <f>SUM(G16:G17)</f>
         <v>598636</v>
       </c>
-      <c r="H34" s="24">
+      <c r="H34" s="71">
         <f>SUM(H16:H17)</f>
         <v>587145</v>
       </c>
-      <c r="I34" s="34">
+      <c r="I34" s="72">
         <f>SUM(I16:I33)</f>
         <v>1377162.81</v>
       </c>
-      <c r="J34" s="35">
+      <c r="J34" s="73">
         <f>J16+J17</f>
         <v>1835021</v>
       </c>
-      <c r="K34" s="26"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="23"/>
-    </row>
-    <row r="35" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="76"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>

</xml_diff>